<commit_message>
update new source in 8thjan
</commit_message>
<xml_diff>
--- a/data/TC002.xlsx
+++ b/data/TC002.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>UserName</t>
   </si>
@@ -27,22 +27,19 @@
     <t>Error Message</t>
   </si>
   <si>
-    <t>password was empty reenter</t>
-  </si>
-  <si>
-    <t>username was empty reenter</t>
-  </si>
-  <si>
-    <t>User not found.</t>
-  </si>
-  <si>
-    <t>Password incorrect.</t>
-  </si>
-  <si>
     <t>gplus.bioemax@gmail.com</t>
   </si>
   <si>
     <t>gplus1.bioemax@gmail.com</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>1234567</t>
+  </si>
+  <si>
+    <t>Ensure valid username/password!</t>
   </si>
 </sst>
 </file>
@@ -108,11 +105,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -418,7 +416,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,42 +438,38 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="2">
-        <v>123456</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2">
-        <v>123456</v>
+        <v>4</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="2">
-        <v>1234567</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New filed updated 12jan
</commit_message>
<xml_diff>
--- a/data/TC002.xlsx
+++ b/data/TC002.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>UserName</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Ensure valid username/password!</t>
+  </si>
+  <si>
+    <t>Ensure valid username/password!s</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +461,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>